<commit_message>
add effects and qol improve.
</commit_message>
<xml_diff>
--- a/Tools/Luban/Datas/Abilities.xlsx
+++ b/Tools/Luban/Datas/Abilities.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90CC8A3-4D5B-4279-AA0B-23126D565C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAB99BD-17CA-4474-9942-4AD396CAD2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="230">
   <si>
     <t>##var</t>
   </si>
@@ -979,11 +979,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>盾牌冷却速度加快25%
--40% 最大护盾</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>FlashShielding</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1021,12 +1016,6 @@
   </si>
   <si>
     <t>RadiantShields</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>+50% 护盾效果半径
-护盾冷却时间延长10%
-最大护盾减少10%</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1086,6 +1075,25 @@
   </si>
   <si>
     <t>盾牌冷却 -20%。</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>盾牌冷却 -25%
+-40% 最大护盾</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>-0.25,-0.4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5,0.1,-0,1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>+50% 护盾效果半径
+护盾冷却时间 +10%
+最大护盾 -10%</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1575,9 +1583,9 @@
   <dimension ref="A1:W100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="F52" sqref="F52"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
@@ -3175,7 +3183,7 @@
         <v>193</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>191</v>
@@ -3211,10 +3219,10 @@
         <v>194</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>195</v>
@@ -3248,7 +3256,7 @@
         <v>197</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E45" s="4">
         <v>0.2</v>
@@ -3314,9 +3322,7 @@
       <c r="W46" s="3"/>
     </row>
     <row r="47" spans="1:23" ht="36.299999999999997" x14ac:dyDescent="0.45">
-      <c r="A47" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="A47" s="3"/>
       <c r="B47" s="3">
         <v>1043</v>
       </c>
@@ -3324,11 +3330,13 @@
         <v>203</v>
       </c>
       <c r="D47" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>204</v>
-      </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4" t="s">
-        <v>205</v>
       </c>
       <c r="G47" s="4">
         <v>1011</v>
@@ -3358,14 +3366,14 @@
         <v>1044</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G48" s="4">
         <v>1011</v>
@@ -3395,14 +3403,14 @@
         <v>1045</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D49" s="11" t="s">
         <v>210</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>211</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G49" s="4">
         <v>1012</v>
@@ -3425,21 +3433,21 @@
       <c r="W49" s="3"/>
     </row>
     <row r="50" spans="1:23" ht="54.45" x14ac:dyDescent="0.45">
-      <c r="A50" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="A50" s="3"/>
       <c r="B50" s="3">
         <v>1046</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F50" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4" t="s">
-        <v>213</v>
       </c>
       <c r="G50" s="4">
         <v>1012</v>
@@ -3469,14 +3477,14 @@
         <v>1047</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G51" s="4">
         <v>1012</v>
@@ -3506,14 +3514,14 @@
         <v>1048</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G52" s="4">
         <v>1012</v>
@@ -5316,7 +5324,7 @@
         <v>198</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F15" s="4">
         <v>1044</v>
@@ -5348,13 +5356,13 @@
         <v>1012</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F16" s="4">
         <v>1048</v>

</xml_diff>

<commit_message>
some bug fix and qol
</commit_message>
<xml_diff>
--- a/Tools/Luban/Datas/Abilities.xlsx
+++ b/Tools/Luban/Datas/Abilities.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA7B1B9-539C-48C6-8862-6C74BF60ED89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFA8C31-C70A-4CCD-87D3-CFA0CDA0B3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12561" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -533,10 +533,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>瞄准</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Targeting</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -714,10 +710,6 @@
   </si>
   <si>
     <t>100,0.1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>添加 100 或 提升 10% 武器瞄准能力</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -955,23 +947,12 @@
 增加 15% 的散布。</t>
   </si>
   <si>
-    <t>武器瞄准 +5%
-+2 子弹
--15% 子弹速度、射速和子弹尺寸
-+75% 武器扩散</t>
-  </si>
-  <si>
     <t>+ 15% 射速</t>
   </si>
   <si>
     <t>武器快速射击，但产生的冷却时间等于射击的累积冷却时间
 +2 连射
 +20% 射速</t>
-  </si>
-  <si>
-    <t>武器瞄准能力 +40%
--20% 子弹总速度
--5% 射速</t>
   </si>
   <si>
     <t>+20% 子弹大小
@@ -1360,13 +1341,6 @@
   </si>
   <si>
     <t>5,1,0.3,0.4,0.1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>发射武器会从侧面发射一对较小的子弹。每发射 5 个子弹，就会额外发射 1 对
-发射的子弹大大提高瞄准能力并且不会很快退化
-发射的子弹的伤害为 30%，速度为 40%
-+10% 武器扩散</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1401,6 +1375,31 @@
   </si>
   <si>
     <t>领导</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>武器追踪能力 +40%
+-20% 子弹总速度
+-5% 射速</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>追踪</t>
+  </si>
+  <si>
+    <t>添加 100 或 提升 10% 武器追踪能力</t>
+  </si>
+  <si>
+    <t>武器追踪 +5%
++2 子弹
+-15% 子弹速度、射速和子弹尺寸
++75% 武器扩散</t>
+  </si>
+  <si>
+    <t>每发射 5 个子弹，就会额外发射 1 对较小的子弹
+额外发射的子弹大大提高追踪能力并且不会很快退化
+额外发射的子弹的伤害为 30%，速度为 40%
++10% 武器扩散</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1925,9 +1924,9 @@
   <dimension ref="A1:W100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
@@ -2141,7 +2140,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E6" s="11">
         <v>-0.15</v>
@@ -2178,7 +2177,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>26</v>
@@ -2208,7 +2207,7 @@
     </row>
     <row r="8" spans="1:23" ht="18.149999999999999" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B8" s="3">
         <v>1004</v>
@@ -2217,7 +2216,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E8" s="11">
         <v>10</v>
@@ -2254,7 +2253,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E9" s="20">
         <v>0.1</v>
@@ -2291,7 +2290,7 @@
         <v>37</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>55</v>
@@ -2321,7 +2320,7 @@
     </row>
     <row r="11" spans="1:23" ht="54.45" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B11" s="3">
         <v>1007</v>
@@ -2330,7 +2329,7 @@
         <v>42</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>58</v>
@@ -2367,10 +2366,10 @@
         <v>43</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>60</v>
@@ -2404,7 +2403,7 @@
         <v>46</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>56</v>
@@ -2471,7 +2470,7 @@
     </row>
     <row r="15" spans="1:23" ht="18.149999999999999" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B15" s="3">
         <v>1011</v>
@@ -2480,10 +2479,10 @@
         <v>51</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>50</v>
@@ -2517,7 +2516,7 @@
         <v>52</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>62</v>
@@ -2554,7 +2553,7 @@
         <v>74</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>76</v>
@@ -2591,7 +2590,7 @@
         <v>78</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>81</v>
@@ -2628,7 +2627,7 @@
         <v>80</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E19" s="4">
         <v>0.15</v>
@@ -2665,7 +2664,7 @@
         <v>82</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E20" s="4">
         <v>-0.3</v>
@@ -2813,7 +2812,7 @@
         <v>97</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E24" s="4">
         <v>0.03</v>
@@ -2847,16 +2846,16 @@
         <v>1021</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="G25" s="4">
         <v>1006</v>
@@ -2884,16 +2883,16 @@
         <v>1022</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>202</v>
+        <v>299</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G26" s="4">
         <v>1006</v>
@@ -2917,22 +2916,22 @@
     </row>
     <row r="27" spans="1:23" ht="72.599999999999994" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B27" s="3">
         <v>1023</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="G27" s="4">
         <v>1006</v>
@@ -2960,16 +2959,16 @@
         <v>1024</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="G28" s="4">
         <v>1006</v>
@@ -2997,16 +2996,16 @@
         <v>1025</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E29" s="4">
         <v>0.2</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G29" s="4">
         <v>1007</v>
@@ -3034,16 +3033,16 @@
         <v>1026</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E30" s="4">
         <v>3</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G30" s="4">
         <v>1007</v>
@@ -3071,16 +3070,16 @@
         <v>1027</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D31" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>123</v>
-      </c>
       <c r="F31" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G31" s="4">
         <v>1007</v>
@@ -3104,22 +3103,22 @@
     </row>
     <row r="32" spans="1:23" ht="72.599999999999994" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B32" s="3">
         <v>1028</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G32" s="4">
         <v>1007</v>
@@ -3143,22 +3142,22 @@
     </row>
     <row r="33" spans="1:23" ht="54.45" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B33" s="3">
         <v>1029</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E33" s="4">
         <v>0.4</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G33" s="4">
         <v>1008</v>
@@ -3182,22 +3181,22 @@
     </row>
     <row r="34" spans="1:23" ht="108.95" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B34" s="3">
         <v>1030</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G34" s="4">
         <v>1008</v>
@@ -3221,22 +3220,22 @@
     </row>
     <row r="35" spans="1:23" ht="36.299999999999997" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B35" s="3">
         <v>1031</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G35" s="4">
         <v>1008</v>
@@ -3264,16 +3263,16 @@
         <v>1032</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E36" s="4">
         <v>0.5</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G36" s="4">
         <v>1008</v>
@@ -3301,16 +3300,16 @@
         <v>1033</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E37" s="4">
         <v>0.25</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G37" s="4">
         <v>1009</v>
@@ -3334,22 +3333,22 @@
     </row>
     <row r="38" spans="1:23" ht="18.149999999999999" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B38" s="3">
         <v>1034</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E38" s="4">
         <v>120</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G38" s="4">
         <v>1009</v>
@@ -3373,22 +3372,22 @@
     </row>
     <row r="39" spans="1:23" ht="90.8" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B39" s="3">
         <v>1035</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G39" s="4">
         <v>1009</v>
@@ -3416,16 +3415,16 @@
         <v>1036</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G40" s="4">
         <v>1009</v>
@@ -3453,16 +3452,16 @@
         <v>1037</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E41" s="4">
         <v>0.2</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G41" s="4">
         <v>1010</v>
@@ -3490,16 +3489,16 @@
         <v>1038</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E42" s="4">
         <v>0.05</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G42" s="4">
         <v>1010</v>
@@ -3527,16 +3526,16 @@
         <v>1039</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G43" s="4">
         <v>1010</v>
@@ -3564,16 +3563,16 @@
         <v>1040</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G44" s="4">
         <v>1010</v>
@@ -3601,16 +3600,16 @@
         <v>1041</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E45" s="4">
         <v>0.2</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G45" s="4">
         <v>1011</v>
@@ -3634,22 +3633,22 @@
     </row>
     <row r="46" spans="1:23" ht="36.299999999999997" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B46" s="3">
         <v>1042</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G46" s="4">
         <v>1011</v>
@@ -3677,16 +3676,16 @@
         <v>1043</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G47" s="4">
         <v>1011</v>
@@ -3714,16 +3713,16 @@
         <v>1044</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G48" s="4">
         <v>1011</v>
@@ -3751,16 +3750,16 @@
         <v>1045</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G49" s="4">
         <v>1012</v>
@@ -3788,16 +3787,16 @@
         <v>1046</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G50" s="4">
         <v>1012</v>
@@ -3825,16 +3824,16 @@
         <v>1047</v>
       </c>
       <c r="C51" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F51" s="4" t="s">
         <v>181</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>183</v>
       </c>
       <c r="G51" s="4">
         <v>1012</v>
@@ -3858,22 +3857,22 @@
     </row>
     <row r="52" spans="1:23" ht="36.299999999999997" x14ac:dyDescent="0.45">
       <c r="A52" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B52" s="3">
         <v>1048</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E52" s="4">
         <v>0.2</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G52" s="4">
         <v>1012</v>
@@ -3897,22 +3896,22 @@
     </row>
     <row r="53" spans="1:23" ht="18.149999999999999" x14ac:dyDescent="0.45">
       <c r="A53" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B53" s="3">
         <v>1049</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E53" s="4">
         <v>0.2</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G53" s="4">
         <v>1013</v>
@@ -3936,22 +3935,22 @@
     </row>
     <row r="54" spans="1:23" ht="18.149999999999999" x14ac:dyDescent="0.45">
       <c r="A54" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B54" s="3">
         <v>1050</v>
       </c>
       <c r="C54" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="D54" s="4" t="s">
-        <v>256</v>
-      </c>
       <c r="E54" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="G54" s="4">
         <v>1013</v>
@@ -3975,22 +3974,22 @@
     </row>
     <row r="55" spans="1:23" ht="18.149999999999999" x14ac:dyDescent="0.45">
       <c r="A55" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B55" s="3">
         <v>1051</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D55" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E55" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="E55" s="4" t="s">
-        <v>258</v>
-      </c>
       <c r="F55" s="4" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="G55" s="4">
         <v>1013</v>
@@ -4014,22 +4013,22 @@
     </row>
     <row r="56" spans="1:23" ht="36.299999999999997" x14ac:dyDescent="0.45">
       <c r="A56" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B56" s="3">
         <v>1052</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="G56" s="4">
         <v>1013</v>
@@ -4053,22 +4052,22 @@
     </row>
     <row r="57" spans="1:23" ht="18.149999999999999" x14ac:dyDescent="0.45">
       <c r="A57" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B57" s="3">
         <v>1053</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="G57" s="4">
         <v>1014</v>
@@ -4092,22 +4091,22 @@
     </row>
     <row r="58" spans="1:23" ht="18.149999999999999" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B58" s="3">
         <v>1054</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E58" s="4">
         <v>0.2</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="G58" s="4">
         <v>1014</v>
@@ -4131,22 +4130,22 @@
     </row>
     <row r="59" spans="1:23" ht="18.149999999999999" x14ac:dyDescent="0.45">
       <c r="A59" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B59" s="3">
         <v>1055</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E59" s="4">
         <v>-0.1</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="G59" s="4">
         <v>1014</v>
@@ -4170,22 +4169,22 @@
     </row>
     <row r="60" spans="1:23" ht="18.149999999999999" x14ac:dyDescent="0.45">
       <c r="A60" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B60" s="3">
         <v>1056</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E60" s="4">
         <v>0.1</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="G60" s="4">
         <v>1014</v>
@@ -5392,7 +5391,7 @@
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
@@ -5419,7 +5418,7 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -5446,10 +5445,10 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="4"/>
@@ -5475,10 +5474,10 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="4"/>
@@ -5504,7 +5503,7 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -5531,7 +5530,7 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -5558,7 +5557,7 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="4"/>
@@ -5585,7 +5584,7 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="4"/>
@@ -5612,7 +5611,7 @@
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -5639,7 +5638,7 @@
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="4"/>
@@ -5666,7 +5665,7 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="4"/>
@@ -5693,7 +5692,7 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -5720,7 +5719,7 @@
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -7933,7 +7932,7 @@
     </row>
     <row r="5" spans="1:26" ht="18.149999999999999" x14ac:dyDescent="0.45">
       <c r="A5" s="22" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B5" s="22">
         <v>1001</v>
@@ -8129,13 +8128,13 @@
         <v>1006</v>
       </c>
       <c r="C10" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="E10" s="25" t="s">
         <v>108</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>109</v>
       </c>
       <c r="F10" s="27">
         <v>1024</v>
@@ -8167,13 +8166,13 @@
         <v>1007</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="25" t="s">
         <v>119</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>120</v>
       </c>
       <c r="F11" s="27">
         <v>1028</v>
@@ -8205,13 +8204,13 @@
         <v>1008</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D12" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" s="25" t="s">
         <v>132</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>133</v>
       </c>
       <c r="F12" s="27">
         <v>1032</v>
@@ -8243,13 +8242,13 @@
         <v>1009</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D13" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13" s="25" t="s">
         <v>138</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>139</v>
       </c>
       <c r="F13" s="27">
         <v>1036</v>
@@ -8281,13 +8280,13 @@
         <v>1010</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F14" s="27">
         <v>1040</v>
@@ -8319,13 +8318,13 @@
         <v>1011</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F15" s="27">
         <v>1044</v>
@@ -8357,13 +8356,13 @@
         <v>1012</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F16" s="27">
         <v>1048</v>
@@ -8391,19 +8390,19 @@
     </row>
     <row r="17" spans="1:26" ht="18.149999999999999" x14ac:dyDescent="0.45">
       <c r="A17" s="28" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B17" s="28">
         <v>1013</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F17" s="30">
         <v>1052</v>
@@ -8435,13 +8434,13 @@
         <v>1014</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F18" s="4">
         <v>1056</v>
@@ -11012,7 +11011,7 @@
         <v>1002</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11">
@@ -11025,7 +11024,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -11052,7 +11051,7 @@
         <v>1003</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="11"/>
@@ -11063,7 +11062,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -11090,10 +11089,10 @@
         <v>1004</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E8" s="11">
         <v>2</v>
@@ -11105,7 +11104,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -13753,16 +13752,16 @@
         <v>9</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
@@ -13871,16 +13870,16 @@
         <v>10</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -13907,11 +13906,11 @@
         <v>1001</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="21" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F5" s="4">
         <v>1000</v>

</xml_diff>